<commit_message>
Fixed decoding, but still need to add data type and map to object, update how the excel file is created to include the series ID codes corresponding names
</commit_message>
<xml_diff>
--- a/src/main/java/decoder_files/smu_decoder_file.xlsx
+++ b/src/main/java/decoder_files/smu_decoder_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\LaborDashboard\src\main\java\decoder_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CB6935-1333-44AE-B5F6-65E14CE26928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4720BCC2-CA4C-44F5-BB23-C78EEB0B9E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="33300" yWindow="4995" windowWidth="11445" windowHeight="11520" xr2:uid="{BF93DD93-9419-4F7C-BCB7-368AC606ADC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF93DD93-9419-4F7C-BCB7-368AC606ADC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2670,7 +2670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2684,6 +2684,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3021,12 +3022,12 @@
   <dimension ref="A1:I448"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>

</xml_diff>